<commit_message>
Adding reporting and logging
</commit_message>
<xml_diff>
--- a/src/test/java/testdata/DriverExcel.xlsx
+++ b/src/test/java/testdata/DriverExcel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\revision\src\test\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2CC2EB-40F1-400E-9D35-D9A791216185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3354F3-AD9C-4D26-AE4F-C52DC731EAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-107" yWindow="-107" windowWidth="24286" windowHeight="15259" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>TcName</t>
   </si>
@@ -61,13 +61,31 @@
   </si>
   <si>
     <t>url</t>
+  </si>
+  <si>
+    <t>TC05</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +95,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,8 +126,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,20 +410,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.8984375" customWidth="1"/>
-    <col min="2" max="2" width="24.69921875" customWidth="1"/>
+    <col min="2" max="2" width="48.09765625" customWidth="1"/>
     <col min="3" max="3" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,8 +433,14 @@
       <c r="C1" t="s">
         <v>10</v>
       </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -419,7 +451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -430,7 +462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -441,7 +473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -450,6 +482,20 @@
       </c>
       <c r="C5" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>